<commit_message>
Blank Menu & Close Button
</commit_message>
<xml_diff>
--- a/OuterAssets/Node Name Gen.xlsx
+++ b/OuterAssets/Node Name Gen.xlsx
@@ -730,7 +730,7 @@
   <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection sqref="A1:A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -747,7 +747,7 @@
       </c>
       <c r="H1" s="3" t="str">
         <f ca="1">CONCATENATE(INDEX(A1:A101, RANDBETWEEN(1, 101)), "'s ", C2)</f>
-        <v>Matthew's Phone</v>
+        <v>Alexander's Phone</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -806,7 +806,7 @@
       </c>
       <c r="H7" s="3" t="str">
         <f ca="1">CONCATENATE(INDEX(A1:A101, RANDBETWEEN(1, 101)), "'s ", C8)</f>
-        <v>Arthur's PC</v>
+        <v>Oscar's Laptop</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -815,14 +815,14 @@
       </c>
       <c r="C8" t="str">
         <f ca="1">INDEX(E7:E10, RANDBETWEEN(1, 4))</f>
-        <v>PC</v>
+        <v>Laptop</v>
       </c>
       <c r="E8" t="s">
         <v>106</v>
       </c>
       <c r="H8" s="3" t="str">
         <f ca="1">CONCATENATE("Terminal ", RANDBETWEEN(1, 100))</f>
-        <v>Terminal 71</v>
+        <v>Terminal 50</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -861,7 +861,7 @@
       </c>
       <c r="H12" s="3" t="str">
         <f ca="1">CONCATENATE(INDEX(A1:A101, RANDBETWEEN(1, 101)), "'s ", C13)</f>
-        <v>Luca's Rig</v>
+        <v>Alfie's Machine</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -870,14 +870,14 @@
       </c>
       <c r="C13" t="str">
         <f ca="1">INDEX(E12:E15, RANDBETWEEN(1, 4))</f>
-        <v>Rig</v>
+        <v>Machine</v>
       </c>
       <c r="E13" t="s">
         <v>108</v>
       </c>
       <c r="H13" s="3" t="str">
         <f ca="1">CONCATENATE("Workstation ", RANDBETWEEN(1, 100))</f>
-        <v>Workstation 88</v>
+        <v>Workstation 43</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -916,7 +916,7 @@
       </c>
       <c r="H17" s="3" t="str">
         <f ca="1">CONCATENATE(INDEX(A1:A101, RANDBETWEEN(1, 101)), "'s ", C18)</f>
-        <v>Poppy's Game Server</v>
+        <v>Sofia's Game Server</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -932,7 +932,7 @@
       </c>
       <c r="H18" s="3" t="str">
         <f ca="1">CONCATENATE("File Server ", RANDBETWEEN(1, 100), ":", RANDBETWEEN(1, 1000))</f>
-        <v>File Server 77:305</v>
+        <v>File Server 71:956</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -941,7 +941,7 @@
       </c>
       <c r="H19" s="3" t="str">
         <f ca="1">CONCATENATE("Research Server ", RANDBETWEEN(10, 99), ":", RANDBETWEEN(100, 999))</f>
-        <v>Research Server 84:659</v>
+        <v>Research Server 21:944</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -959,7 +959,7 @@
       </c>
       <c r="H21" s="3" t="str">
         <f ca="1">CONCATENATE("Array ", CHAR(RANDBETWEEN(65, 90)), RANDBETWEEN(100, 999))</f>
-        <v>Array K836</v>
+        <v>Array M922</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -977,7 +977,7 @@
       </c>
       <c r="H23" s="3" t="str">
         <f ca="1">CONCATENATE(CHAR(RANDBETWEEN(65, 90)), CHAR(RANDBETWEEN(65, 90)), RANDBETWEEN(100, 999))</f>
-        <v>CX387</v>
+        <v>TR647</v>
       </c>
     </row>
     <row r="24" spans="1:8">

</xml_diff>